<commit_message>
Update BCRPP Correction Rules.xlsx
removing correction rule checks we don't want to do
</commit_message>
<xml_diff>
--- a/BCRPP_QC_R_Excel_Program/Core QC Rules/BCRPP Correction Rules.xlsx
+++ b/BCRPP_QC_R_Excel_Program/Core QC Rules/BCRPP Correction Rules.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C83AE2B-0137-4D43-B6E2-593F401DA7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D2A28D-62AD-BC4C-88FA-FDC9A12CFD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40960" yWindow="800" windowWidth="40960" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="128">
   <si>
     <t>variable</t>
   </si>
@@ -103,9 +103,6 @@
     <t>parity &gt;= 1</t>
   </si>
   <si>
-    <t>age_preg1 changed to 888 from 777 (parous is 1 and Parity &gt;= 1 )</t>
-  </si>
-  <si>
     <t>age_preg2 %in% c(666,777)</t>
   </si>
   <si>
@@ -160,12 +157,6 @@
     <t>parity ==888</t>
   </si>
   <si>
-    <t>age_preg1 changed to 888 from 777 (parous is 888 and parity == 888 )</t>
-  </si>
-  <si>
-    <t>age_preg2 changed to 888 from 666 or 777 (parous is 888 and parity == 888)</t>
-  </si>
-  <si>
     <t>age_preg2 changed to 888 from 666 or 777 (parous is 1 and parity &gt;= 2)</t>
   </si>
   <si>
@@ -184,33 +175,12 @@
     <t>age_preg7 changed to 888 from 666 or 777 (parous is 1 and parity &gt;= 7)</t>
   </si>
   <si>
-    <t>age_preg3 changed to 888 from 666 or 777 (parous is 888 and parity == 888)</t>
-  </si>
-  <si>
-    <t>age_preg4 changed to 888 from 666 or 777 (parous is 888 and parity == 888)</t>
-  </si>
-  <si>
-    <t>age_preg5 changed to 888 from 666 or 777 (parous is 888 and parity == 888)</t>
-  </si>
-  <si>
-    <t>age_preg6 changed to 888 from 666 or 777 (parous is 888 and parity == 888)</t>
-  </si>
-  <si>
-    <t>age_preg7 changed to 888 from 666 or 777 (parous is 888 and parity == 888)</t>
-  </si>
-  <si>
     <t>agemenarche</t>
   </si>
   <si>
     <t>agemenarche to 888 from 777 (777 is not an acceptable value)</t>
   </si>
   <si>
-    <t>alcohol_amt</t>
-  </si>
-  <si>
-    <t>alcohol_amt changed to 888 from 777 (777 is not an acceptable value)</t>
-  </si>
-  <si>
     <t>BBD_history</t>
   </si>
   <si>
@@ -229,66 +199,27 @@
     <t>BBD_number changed to 0 from 777/888 (BBD_history is 0 )</t>
   </si>
   <si>
-    <t>1, 888</t>
-  </si>
-  <si>
     <t>BBD_type1</t>
   </si>
   <si>
-    <t>0, 777</t>
-  </si>
-  <si>
-    <t>BBD_number changed to 888 from 0/777 ( BBD_history is 1 or 888)</t>
-  </si>
-  <si>
     <t>crossvalid2.changes</t>
   </si>
   <si>
-    <t xml:space="preserve">1, 888 </t>
-  </si>
-  <si>
-    <t>BBD_type1 changed to 888 from 777 (BBD_history is 888 and BBD_number is 1 or 888)</t>
-  </si>
-  <si>
     <t>BBD_type2</t>
   </si>
   <si>
-    <t>2, 888</t>
-  </si>
-  <si>
-    <t>BBD_type2 changed to 888 from 777 (BBD_history is 1 or 888 and BBD_number is 2 or 888)</t>
-  </si>
-  <si>
     <t>BBD_type3</t>
   </si>
   <si>
-    <t>3, 888</t>
-  </si>
-  <si>
-    <t>BBD_type3 changed to 888 from 777 (BBD_history is 1 or 888 and BBD_number is 3 or 888)</t>
-  </si>
-  <si>
     <t>BBD_type4</t>
   </si>
   <si>
-    <t>4, 888</t>
-  </si>
-  <si>
-    <t>BBD_type4 changed to 888 from 777 (BBD_history is 1 or 888 and BBD_number is 4 or 888)</t>
-  </si>
-  <si>
     <t>Biopsies_yesno</t>
   </si>
   <si>
     <t>Biopsies_yesno changed to 888 from 777 (777 is not an acceptable value)</t>
   </si>
   <si>
-    <t>Biopsies_number</t>
-  </si>
-  <si>
-    <t>Biopsies_number changed to 888 from 777 (777 is not an acceptable value)</t>
-  </si>
-  <si>
     <t>bmi</t>
   </si>
   <si>
@@ -316,24 +247,15 @@
     <t>age_preg8 %in% c(666,777)</t>
   </si>
   <si>
-    <t>age_preg8 changed to 888 from 666 or 777 (parous is 888 and parity == 888)</t>
-  </si>
-  <si>
     <t>age_preg9</t>
   </si>
   <si>
     <t>age_preg9 %in% c(666,777)</t>
   </si>
   <si>
-    <t>age_preg9 changed to 888 from 666 or 777 (parous is 888 and parity == 888)</t>
-  </si>
-  <si>
     <t>age_preg10</t>
   </si>
   <si>
-    <t>age_preg10 changed to 888 from 666 or 777 (parous is 888 and parity == 888)</t>
-  </si>
-  <si>
     <t>parity &gt;= 8</t>
   </si>
   <si>
@@ -361,15 +283,9 @@
     <t>0, 1</t>
   </si>
   <si>
-    <t>breastfeed changed from 0 or 1 to 777 (parous is 0, parity is 0, age_preg1 is 777 )</t>
-  </si>
-  <si>
     <t>0, 888</t>
   </si>
   <si>
-    <t>breastfeed changed to 777 from 0/888 ( parous is 0, parity is 0 and age_preg1 is 777 )</t>
-  </si>
-  <si>
     <t>breastfeed_dur</t>
   </si>
   <si>
@@ -430,19 +346,77 @@
     <t>100 * height</t>
   </si>
   <si>
-    <t>height converted to centimeters from meters (meters multiplied by 100 )</t>
-  </si>
-  <si>
     <t>height changed to 888 from 777 (777 is not an acceptable value)</t>
+  </si>
+  <si>
+    <t>age_preg1 changed to 888 from 777 (parous is 1 and parity &gt;= 1 )</t>
+  </si>
+  <si>
+    <t>age_preg1 changed to 888 from 777 (parous is 888 and parity is 888 )</t>
+  </si>
+  <si>
+    <t>age_preg2 changed to 888 from 666 or 777 (parous is 888 and parity is 888)</t>
+  </si>
+  <si>
+    <t>age_preg3 changed to 888 from 666 or 777 (parous is 888 and parity is 888)</t>
+  </si>
+  <si>
+    <t>age_preg4 changed to 888 from 666 or 777 (parous is 888 and parity is 888)</t>
+  </si>
+  <si>
+    <t>age_preg5 changed to 888 from 666 or 777 (parous is 888 and parity is 888)</t>
+  </si>
+  <si>
+    <t>age_preg6 changed to 888 from 666 or 777 (parous is 888 and parity is 888)</t>
+  </si>
+  <si>
+    <t>age_preg7 changed to 888 from 666 or 777 (parous is 888 and parity is 888)</t>
+  </si>
+  <si>
+    <t>age_preg8 changed to 888 from 666 or 777 (parous is 888 and parity is 888)</t>
+  </si>
+  <si>
+    <t>age_preg9 changed to 888 from 666 or 777 (parous is 888 and parity is 888)</t>
+  </si>
+  <si>
+    <t>age_preg10 changed to 888 from 666 or 777 (parous is 888 and parity is 888)</t>
+  </si>
+  <si>
+    <t>BBD_type1 changed to 888 from 777 (BBD_history is 1 and BBD_number is 1)</t>
+  </si>
+  <si>
+    <t>BBD_type2 changed to 888 from 777 (BBD_history is 1 and BBD_number is 2)</t>
+  </si>
+  <si>
+    <t>BBD_type3 changed to 888 from 777 (BBD_history is 1 and BBD_number is 3)</t>
+  </si>
+  <si>
+    <t>BBD_type4 changed to 888 from 777 (BBD_history is 1 and BBD_number is 4)</t>
+  </si>
+  <si>
+    <t>breastfeed changed from 0 or 1 to 777 (parous is 0, parity is 0, age_preg1 is 777)</t>
+  </si>
+  <si>
+    <t>breastfeed changed to 777 from 0/888 ( parous is 0, parity is 0 and age_preg1 is 777)</t>
+  </si>
+  <si>
+    <t>height converted to centimeters from meters (meters multiplied by 100)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -503,10 +477,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -813,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O41" sqref="A41:XFD41"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -920,8 +895,8 @@
       <c r="L3" s="1">
         <v>888</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>28</v>
+      <c r="M3" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -929,7 +904,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>25</v>
@@ -944,13 +919,13 @@
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L4" s="1">
         <v>888</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -958,7 +933,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>25</v>
@@ -973,21 +948,21 @@
         <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L5" s="1">
         <v>888</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>25</v>
@@ -1002,21 +977,21 @@
         <v>20</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L6" s="1">
         <v>888</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>25</v>
@@ -1031,21 +1006,21 @@
         <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L7" s="1">
         <v>888</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>25</v>
@@ -1060,21 +1035,21 @@
         <v>20</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L8" s="1">
         <v>888</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>25</v>
@@ -1089,21 +1064,21 @@
         <v>20</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L9" s="1">
         <v>888</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>25</v>
@@ -1118,21 +1093,21 @@
         <v>20</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="L10" s="1">
         <v>888</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>25</v>
@@ -1147,21 +1122,21 @@
         <v>20</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="L11" s="1">
         <v>888</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
@@ -1176,13 +1151,13 @@
         <v>20</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="L12" s="1">
         <v>888</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1199,19 +1174,19 @@
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="L13" s="1">
         <v>888</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>47</v>
+      <c r="M13" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1219,7 +1194,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>25</v>
@@ -1228,19 +1203,19 @@
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="L14" s="1">
         <v>888</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>48</v>
+      <c r="M14" s="5" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1248,7 +1223,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>25</v>
@@ -1257,28 +1232,28 @@
         <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="L15" s="1">
         <v>888</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>55</v>
+      <c r="M15" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1286,27 +1261,27 @@
         <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="L16" s="1">
         <v>888</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>56</v>
+      <c r="M16" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>25</v>
@@ -1315,27 +1290,27 @@
         <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="L17" s="1">
         <v>888</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>57</v>
+      <c r="M17" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>25</v>
@@ -1344,28 +1319,28 @@
         <v>14</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="L18" s="1">
         <v>888</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>58</v>
+      <c r="M18" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="C19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1373,27 +1348,27 @@
         <v>14</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="L19" s="1">
         <v>888</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>59</v>
+      <c r="M19" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>25</v>
@@ -1402,27 +1377,27 @@
         <v>14</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="L20" s="1">
         <v>888</v>
       </c>
-      <c r="M20" s="1" t="s">
-        <v>99</v>
+      <c r="M20" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>25</v>
@@ -1431,13 +1406,13 @@
         <v>14</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1447,15 +1422,15 @@
         <v>888</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>25</v>
@@ -1464,13 +1439,13 @@
         <v>14</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1480,7 +1455,7 @@
         <v>888</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -1491,7 +1466,7 @@
         <v>777</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>14</v>
@@ -1513,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -1524,7 +1499,7 @@
         <v>777</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>14</v>
@@ -1546,12 +1521,12 @@
         <v>888</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1">
         <v>777</v>
@@ -1563,12 +1538,12 @@
         <v>888</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="B26" s="1">
         <v>777</v>
@@ -1580,12 +1555,12 @@
         <v>888</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B27" s="1">
         <v>777</v>
@@ -1597,464 +1572,407 @@
         <v>888</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="1">
-        <v>777</v>
+        <v>56</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>16</v>
+        <v>58</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
       </c>
       <c r="L28" s="1">
-        <v>888</v>
+        <v>0</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
+      </c>
+      <c r="B29" s="1">
+        <v>777</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="E29" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
       </c>
       <c r="L29" s="1">
-        <v>0</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>69</v>
+        <v>888</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
+      </c>
+      <c r="B30" s="1">
+        <v>777</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2</v>
       </c>
       <c r="L30" s="1">
         <v>888</v>
       </c>
-      <c r="M30" s="1" t="s">
-        <v>73</v>
+      <c r="M30" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B31" s="1">
         <v>777</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>75</v>
+        <v>54</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
+      </c>
+      <c r="G31" s="1">
+        <v>3</v>
       </c>
       <c r="L31" s="1">
         <v>888</v>
       </c>
-      <c r="M31" s="1" t="s">
-        <v>76</v>
+      <c r="M31" s="5" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B32" s="1">
         <v>777</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>75</v>
+        <v>54</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>78</v>
+        <v>56</v>
+      </c>
+      <c r="G32" s="1">
+        <v>4</v>
       </c>
       <c r="L32" s="1">
         <v>888</v>
       </c>
-      <c r="M32" s="1" t="s">
-        <v>79</v>
+      <c r="M32" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B33" s="1">
         <v>777</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L33" s="1">
+        <v>888</v>
+      </c>
+      <c r="M33" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L33" s="1">
-        <v>888</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B34" s="1">
-        <v>777</v>
+        <v>67</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>64</v>
+        <v>25</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L34" s="1">
-        <v>888</v>
+        <v>71</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>86</v>
+      <c r="A35" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B35" s="1">
         <v>777</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G35" s="3"/>
       <c r="L35" s="1">
         <v>888</v>
       </c>
-      <c r="M35" s="2" t="s">
-        <v>87</v>
+      <c r="M35" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" s="1">
-        <v>777</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L36" s="1">
-        <v>888</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>89</v>
+      <c r="A36" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>96</v>
+      <c r="A37" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="L37" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38" s="1">
+        <v>69</v>
+      </c>
+      <c r="B38" s="4">
         <v>777</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="3"/>
-      <c r="L38" s="1">
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="L38" s="4">
         <v>888</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D39" s="4" t="s">
+      <c r="A39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" s="1">
+        <v>777</v>
+      </c>
+      <c r="L39" s="1">
+        <v>777</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="1">
+        <v>777</v>
+      </c>
+      <c r="L40" s="1">
+        <v>777</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L41" s="1">
+        <v>888</v>
+      </c>
+      <c r="M41" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="L39" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="M39" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="L40" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="M40" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41" s="4">
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42" s="1">
         <v>777</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="L41" s="4">
-        <v>888</v>
-      </c>
-      <c r="M41" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E42" s="1">
-        <v>0</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G42" s="1">
-        <v>0</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I42" s="1">
-        <v>777</v>
-      </c>
       <c r="L42" s="1">
-        <v>777</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E43" s="1">
-        <v>0</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G43" s="1">
-        <v>0</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I43" s="1">
-        <v>777</v>
-      </c>
-      <c r="L43" s="1">
-        <v>777</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="L44" s="1">
-        <v>888</v>
-      </c>
-      <c r="M44" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B45" s="1">
-        <v>777</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L45" s="1">
-        <v>888</v>
-      </c>
-      <c r="M45" s="4" t="s">
-        <v>127</v>
+        <v>888</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>